<commit_message>
sua lai layout code tiếp màn quản lý sản phẩm
</commit_message>
<xml_diff>
--- a/App_View/wwwroot/ImportErrors.xlsx
+++ b/App_View/wwwroot/ImportErrors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Tên SP</t>
   </si>
@@ -65,10 +65,13 @@
     <t>Mô tả lỗi</t>
   </si>
   <si>
-    <t>Impact 4</t>
-  </si>
-  <si>
-    <t>Nike</t>
+    <t>01a9bd40-978a-46ab-85ed-9d603452834e</t>
+  </si>
+  <si>
+    <t>HEAWYN</t>
+  </si>
+  <si>
+    <t>Adidas</t>
   </si>
   <si>
     <t>Đức</t>
@@ -77,67 +80,31 @@
     <t>Da</t>
   </si>
   <si>
-    <t>Giày bóng rổ</t>
+    <t>Giày chạy bộ</t>
   </si>
   <si>
     <t>Đế đinh</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>43</t>
+    <t>white</t>
+  </si>
+  <si>
+    <t>550</t>
   </si>
   <si>
     <t>2400000</t>
   </si>
   <si>
-    <t>4700000</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>Impact_4_blue1.png,Impact_4_blue2.png,Impact_4_blue3.png,Impact_4_blue4.png</t>
-  </si>
-  <si>
-    <t>Sản phẩm đã tồn tại</t>
-  </si>
-  <si>
-    <t>Air Max 90</t>
-  </si>
-  <si>
-    <t>Trung Quốc</t>
-  </si>
-  <si>
-    <t>Men's Shoes</t>
-  </si>
-  <si>
-    <t>Đế phẳng</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>3000000</t>
-  </si>
-  <si>
-    <t>5600000</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Air_Max _90_black_1.png,Air_Max _90_black_2.png,Air_Max _90_black_3.png,Air_Max _90_black_4.png</t>
+    <t>550000</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sai định dạng hoặc để trống trường</t>
   </si>
 </sst>
 </file>
@@ -191,7 +158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -288,10 +255,10 @@
         <v>28</v>
       </c>
       <c r="M2" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="0" t="b">
         <v>1</v>
@@ -300,59 +267,6 @@
         <v>29</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="O3" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="0" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sửa lại màn Sale
</commit_message>
<xml_diff>
--- a/App_View/wwwroot/ImportErrors.xlsx
+++ b/App_View/wwwroot/ImportErrors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Tên SP</t>
   </si>
@@ -101,7 +101,7 @@
     <t>160</t>
   </si>
   <si>
-    <t/>
+    <t>Impact_4_blue1.png,Impact_4_blue2.png,Impact_4_blue3.png,Impact_4_blue4.png</t>
   </si>
   <si>
     <t>Sản phẩm đã tồn tại</t>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>34</t>
+  </si>
+  <si>
+    <t>Air_Max _90_black_1.png,Air_Max _90_black_2.png,Air_Max _90_black_3.png,Air_Max _90_black_4.png</t>
   </si>
 </sst>
 </file>
@@ -291,7 +294,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>29</v>
@@ -344,10 +347,10 @@
         <v>1</v>
       </c>
       <c r="O3" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>30</v>

</xml_diff>